<commit_message>
Complete un poco la cuadricula
</commit_message>
<xml_diff>
--- a/DATOS/Boceto de cuadriculas.xlsx
+++ b/DATOS/Boceto de cuadriculas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fede\Desktop\PROGRAMACION\JAVASCRIPT\Proyectos\Porcentaje de Ventas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Fede\Desktop\PROGRAMACION\JAVASCRIPT\Proyectos\Balance de Remeras\DATOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>#4</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>(Gastos totales</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>Última tirada</t>
   </si>
 </sst>
 </file>
@@ -533,10 +539,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:J17"/>
+  <dimension ref="C4:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="I5:J10"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,12 +550,13 @@
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" customWidth="1"/>
-    <col min="7" max="7" width="35.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
+    <col min="8" max="8" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
@@ -562,7 +569,7 @@
       </c>
       <c r="J5" s="3"/>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C6" s="10" t="s">
         <v>9</v>
       </c>
@@ -576,12 +583,18 @@
         <v>11</v>
       </c>
       <c r="G6" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="4"/>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="K6" s="4"/>
+      <c r="L6" s="5"/>
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C7" s="11" t="s">
         <v>14</v>
       </c>
@@ -595,14 +608,16 @@
         <v>12</v>
       </c>
       <c r="G7" s="11"/>
-      <c r="I7" s="9" t="s">
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="K7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="L7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C8" s="11" t="s">
         <v>15</v>
       </c>
@@ -616,14 +631,16 @@
         <v>12</v>
       </c>
       <c r="G8" s="11"/>
-      <c r="I8" s="4" t="s">
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="K8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C9" s="11" t="s">
         <v>16</v>
       </c>
@@ -637,14 +654,16 @@
         <v>12</v>
       </c>
       <c r="G9" s="11"/>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+      <c r="K9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C10" s="11" t="s">
         <v>0</v>
       </c>
@@ -658,14 +677,16 @@
         <v>12</v>
       </c>
       <c r="G10" s="11"/>
-      <c r="I10" s="4" t="s">
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="K10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C11" s="11" t="s">
         <v>1</v>
       </c>
@@ -675,10 +696,12 @@
         <v>12</v>
       </c>
       <c r="G11" s="11"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="5"/>
-    </row>
-    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+      <c r="K11" s="4"/>
+      <c r="L11" s="5"/>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C12" s="11" t="s">
         <v>2</v>
       </c>
@@ -688,10 +711,12 @@
         <v>12</v>
       </c>
       <c r="G12" s="11"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="5"/>
-    </row>
-    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+      <c r="K12" s="4"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C13" s="11" t="s">
         <v>3</v>
       </c>
@@ -701,10 +726,12 @@
         <v>12</v>
       </c>
       <c r="G13" s="11"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="5"/>
-    </row>
-    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+      <c r="K13" s="4"/>
+      <c r="L13" s="5"/>
+    </row>
+    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C14" s="11" t="s">
         <v>4</v>
       </c>
@@ -714,10 +741,12 @@
         <v>12</v>
       </c>
       <c r="G14" s="11"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="5"/>
-    </row>
-    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+      <c r="K14" s="4"/>
+      <c r="L14" s="5"/>
+    </row>
+    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C15" s="11" t="s">
         <v>5</v>
       </c>
@@ -727,10 +756,12 @@
         <v>12</v>
       </c>
       <c r="G15" s="11"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="5"/>
-    </row>
-    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
       <c r="C16" s="11" t="s">
         <v>6</v>
       </c>
@@ -740,8 +771,10 @@
         <v>12</v>
       </c>
       <c r="G16" s="11"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="5"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="5"/>
     </row>
     <row r="17" spans="9:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="I17" s="7"/>

</xml_diff>